<commit_message>
final forecasts + report
</commit_message>
<xml_diff>
--- a/2. extension/MAE.xlsx
+++ b/2. extension/MAE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeann\OneDrive\Documents\scolaire\ENSAE\3A\S1\macroeconometrics and ML\project\Macroeconometrics-and-Machine-Learning-Project\2. extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDD8204-5CED-4246-972D-01103EA39127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0AB678-7702-43B0-BCBD-0E832CAE3674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10830" yWindow="450" windowWidth="9825" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>adaElNet.rda</t>
   </si>
@@ -37,6 +37,9 @@
     <t>BVAR.rda</t>
   </si>
   <si>
+    <t>CSR.rda</t>
+  </si>
+  <si>
     <t>ElNet.rda</t>
   </si>
   <si>
@@ -49,6 +52,9 @@
     <t>RF.rda</t>
   </si>
   <si>
+    <t>RFOLS.rda</t>
+  </si>
+  <si>
     <t>Ridge.rda</t>
   </si>
   <si>
@@ -57,66 +63,12 @@
   <si>
     <t>is_min</t>
   </si>
-  <si>
-    <t>t+1</t>
-  </si>
-  <si>
-    <t>t+2</t>
-  </si>
-  <si>
-    <t>t+3</t>
-  </si>
-  <si>
-    <t>t+4</t>
-  </si>
-  <si>
-    <t>t+5</t>
-  </si>
-  <si>
-    <t>t+6</t>
-  </si>
-  <si>
-    <t>t+7</t>
-  </si>
-  <si>
-    <t>t+8</t>
-  </si>
-  <si>
-    <t>t+9</t>
-  </si>
-  <si>
-    <t>t+10</t>
-  </si>
-  <si>
-    <t>t+11</t>
-  </si>
-  <si>
-    <t>t+12</t>
-  </si>
-  <si>
-    <t>acc3</t>
-  </si>
-  <si>
-    <t>acc6</t>
-  </si>
-  <si>
-    <t>acc12</t>
-  </si>
-  <si>
-    <t>avg</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,12 +80,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -512,73 +458,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.39234487976493931</v>
+      </c>
       <c r="B2">
-        <v>0.39234487976493931</v>
+        <v>0.46234983006153679</v>
       </c>
       <c r="C2">
-        <v>0.46234983006153679</v>
+        <v>1.0171733480363669</v>
       </c>
       <c r="D2">
-        <v>1.0171733480363669</v>
+        <v>0.25198495601383319</v>
       </c>
       <c r="E2">
-        <v>0.43805632942462702</v>
+        <v>1.0046438909176461</v>
       </c>
       <c r="F2">
-        <v>1.0046438909176461</v>
+        <v>0.64780664634315088</v>
       </c>
       <c r="G2">
         <v>0.1243332478882081</v>
@@ -587,39 +539,42 @@
         <v>0.8525777542776477</v>
       </c>
       <c r="I2">
-        <v>0.46234983006153679</v>
+        <v>0.1174010591161055</v>
       </c>
       <c r="J2">
         <v>1.187554308096719</v>
       </c>
       <c r="K2">
+        <v>0.29646130615408012</v>
+      </c>
+      <c r="L2">
         <v>2.9940191417630619</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.69000445657469534</v>
       </c>
       <c r="B3">
-        <v>0.69000445657469534</v>
+        <v>0.70258061602849675</v>
       </c>
       <c r="C3">
-        <v>0.70258061602849675</v>
+        <v>1.0323587950046531</v>
       </c>
       <c r="D3">
-        <v>1.0323587950046531</v>
+        <v>1.2339849803223031</v>
       </c>
       <c r="E3">
-        <v>1.177224083861814</v>
+        <v>1.0131648701625111</v>
       </c>
       <c r="F3">
-        <v>1.0131648701625111</v>
+        <v>0.92528884182705617</v>
       </c>
       <c r="G3">
         <v>0.77858592797786352</v>
@@ -628,39 +583,42 @@
         <v>0.91940977140149305</v>
       </c>
       <c r="I3">
-        <v>0.70258061602849675</v>
+        <v>0.70942440303719534</v>
       </c>
       <c r="J3">
         <v>1.1721661156957981</v>
       </c>
       <c r="K3">
+        <v>0.89106829606102522</v>
+      </c>
+      <c r="L3">
         <v>1.99164018634794</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.91651801129583366</v>
       </c>
       <c r="B4">
-        <v>0.91651801129583366</v>
+        <v>0.88232489121805535</v>
       </c>
       <c r="C4">
-        <v>0.88232489121805535</v>
+        <v>1.048802755805063</v>
       </c>
       <c r="D4">
-        <v>1.048802755805063</v>
+        <v>1.8501042166790329</v>
       </c>
       <c r="E4">
-        <v>2.5453516254334758</v>
+        <v>1.0182368562137569</v>
       </c>
       <c r="F4">
-        <v>1.0182368562137569</v>
+        <v>1.041189499488421</v>
       </c>
       <c r="G4">
         <v>1.0125808303657371</v>
@@ -669,39 +627,42 @@
         <v>0.90944655761177207</v>
       </c>
       <c r="I4">
-        <v>0.88232489121805535</v>
+        <v>0.92888518349118798</v>
       </c>
       <c r="J4">
         <v>1.147060420862118</v>
       </c>
       <c r="K4">
+        <v>1.2443168862495251</v>
+      </c>
+      <c r="L4">
         <v>1.5557501030683309</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.119775096089614</v>
       </c>
       <c r="B5">
-        <v>1.119775096089614</v>
+        <v>1.100884940767497</v>
       </c>
       <c r="C5">
-        <v>1.100884940767497</v>
+        <v>1.059064424309327</v>
       </c>
       <c r="D5">
-        <v>1.059064424309327</v>
+        <v>2.3916467679167739</v>
       </c>
       <c r="E5">
-        <v>4.0073072959965126</v>
+        <v>1.047051221672213</v>
       </c>
       <c r="F5">
-        <v>1.047051221672213</v>
+        <v>1.1691020379484329</v>
       </c>
       <c r="G5">
         <v>1.1688072997444641</v>
@@ -710,39 +671,42 @@
         <v>0.97901925013612379</v>
       </c>
       <c r="I5">
-        <v>1.100884940767497</v>
+        <v>1.1124360829309099</v>
       </c>
       <c r="J5">
         <v>1.1145555129873641</v>
       </c>
       <c r="K5">
+        <v>1.4700721975850159</v>
+      </c>
+      <c r="L5">
         <v>1.3735285686523939</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.219974302028346</v>
       </c>
       <c r="B6">
-        <v>1.219974302028346</v>
+        <v>1.1569221633602129</v>
       </c>
       <c r="C6">
-        <v>1.1569221633602129</v>
+        <v>1.076022915601285</v>
       </c>
       <c r="D6">
-        <v>1.076022915601285</v>
+        <v>3.1907983295295641</v>
       </c>
       <c r="E6">
-        <v>2.5362796415169679</v>
+        <v>1.060699982094635</v>
       </c>
       <c r="F6">
-        <v>1.060699982094635</v>
+        <v>1.1875406449131289</v>
       </c>
       <c r="G6">
         <v>1.2122338366242931</v>
@@ -751,39 +715,42 @@
         <v>0.99237806417084351</v>
       </c>
       <c r="I6">
-        <v>1.1569221633602129</v>
+        <v>1.1550468761084101</v>
       </c>
       <c r="J6">
         <v>1.0318442685980449</v>
       </c>
       <c r="K6">
+        <v>1.4914164883076479</v>
+      </c>
+      <c r="L6">
         <v>1.247326043973279</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.1390433143729859</v>
       </c>
       <c r="B7">
-        <v>1.1390433143729859</v>
+        <v>1.0079764048419459</v>
       </c>
       <c r="C7">
-        <v>1.0079764048419459</v>
+        <v>1.068586720473399</v>
       </c>
       <c r="D7">
-        <v>1.068586720473399</v>
+        <v>3.321215749099343</v>
       </c>
       <c r="E7">
-        <v>2.5906215473427552</v>
+        <v>1.0577962961482601</v>
       </c>
       <c r="F7">
-        <v>1.0577962961482601</v>
+        <v>1.1220071035752861</v>
       </c>
       <c r="G7">
         <v>1.2052426045839939</v>
@@ -792,39 +759,42 @@
         <v>0.9777558611633842</v>
       </c>
       <c r="I7">
-        <v>1.0079764048419459</v>
+        <v>1.0242311663505419</v>
       </c>
       <c r="J7">
         <v>0.97802413452545489</v>
       </c>
       <c r="K7">
+        <v>1.3230891857946101</v>
+      </c>
+      <c r="L7">
         <v>1.1283054841128459</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.161243009242064</v>
       </c>
       <c r="B8">
-        <v>1.161243009242064</v>
+        <v>1.2019809017919409</v>
       </c>
       <c r="C8">
-        <v>1.2019809017919409</v>
+        <v>1.0586210361275821</v>
       </c>
       <c r="D8">
-        <v>1.0586210361275821</v>
+        <v>3.309095571398001</v>
       </c>
       <c r="E8">
-        <v>3.3265317961218379</v>
+        <v>1.0475858495496591</v>
       </c>
       <c r="F8">
-        <v>1.0475858495496591</v>
+        <v>1.0915881184145759</v>
       </c>
       <c r="G8">
         <v>1.13709800527215</v>
@@ -833,39 +803,42 @@
         <v>0.94423196724223102</v>
       </c>
       <c r="I8">
-        <v>1.2019809017919409</v>
+        <v>1.1690985507636129</v>
       </c>
       <c r="J8">
         <v>0.94472511912981127</v>
       </c>
       <c r="K8">
+        <v>1.1974126492285491</v>
+      </c>
+      <c r="L8">
         <v>1.0423440520712619</v>
       </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1.140148694883415</v>
       </c>
       <c r="B9">
-        <v>1.140148694883415</v>
+        <v>1.2094150890960329</v>
       </c>
       <c r="C9">
-        <v>1.2094150890960329</v>
+        <v>1.027671865060666</v>
       </c>
       <c r="D9">
-        <v>1.027671865060666</v>
+        <v>2.8724879665856031</v>
       </c>
       <c r="E9">
-        <v>2.9583372834308221</v>
+        <v>1.028384974482206</v>
       </c>
       <c r="F9">
-        <v>1.028384974482206</v>
+        <v>1.079806859677418</v>
       </c>
       <c r="G9">
         <v>1.0564883646356851</v>
@@ -874,39 +847,42 @@
         <v>0.93888982033379242</v>
       </c>
       <c r="I9">
-        <v>1.2094150890960329</v>
+        <v>1.1126979433935571</v>
       </c>
       <c r="J9">
         <v>0.94744596827977523</v>
       </c>
       <c r="K9">
+        <v>1.208453916334026</v>
+      </c>
+      <c r="L9">
         <v>0.98476270175444081</v>
       </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1.137063311018669</v>
       </c>
       <c r="B10">
-        <v>1.137063311018669</v>
+        <v>1.2190641998303879</v>
       </c>
       <c r="C10">
-        <v>1.2190641998303879</v>
+        <v>1.0161747308691931</v>
       </c>
       <c r="D10">
-        <v>1.0161747308691931</v>
+        <v>3.769871237702251</v>
       </c>
       <c r="E10">
-        <v>3.7594387654622881</v>
+        <v>1.0246482618238679</v>
       </c>
       <c r="F10">
-        <v>1.0246482618238679</v>
+        <v>1.0456685122427669</v>
       </c>
       <c r="G10">
         <v>1.049989425861388</v>
@@ -915,39 +891,42 @@
         <v>0.9328597783451329</v>
       </c>
       <c r="I10">
-        <v>1.2190641998303879</v>
+        <v>1.1152911553665219</v>
       </c>
       <c r="J10">
         <v>0.95865736128570234</v>
       </c>
       <c r="K10">
+        <v>1.231630093430532</v>
+      </c>
+      <c r="L10">
         <v>0.94615474379672515</v>
       </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1.0952281477996419</v>
       </c>
       <c r="B11">
-        <v>1.0952281477996419</v>
+        <v>1.1898870292029731</v>
       </c>
       <c r="C11">
-        <v>1.1898870292029731</v>
+        <v>1.005118722302426</v>
       </c>
       <c r="D11">
-        <v>1.005118722302426</v>
+        <v>2.1357159141933679</v>
       </c>
       <c r="E11">
-        <v>2.2020510130602502</v>
+        <v>1.0108330382125379</v>
       </c>
       <c r="F11">
-        <v>1.0108330382125379</v>
+        <v>0.9923158600027705</v>
       </c>
       <c r="G11">
         <v>1.038036134990155</v>
@@ -956,39 +935,42 @@
         <v>0.92569103471168601</v>
       </c>
       <c r="I11">
-        <v>1.1898870292029731</v>
+        <v>1.0919348605254651</v>
       </c>
       <c r="J11">
         <v>0.9862687402225212</v>
       </c>
       <c r="K11">
+        <v>1.245918553134046</v>
+      </c>
+      <c r="L11">
         <v>0.91055752063775885</v>
       </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.95212907631401578</v>
       </c>
       <c r="B12">
-        <v>0.95212907631401578</v>
+        <v>0.96489092907264762</v>
       </c>
       <c r="C12">
-        <v>0.96489092907264762</v>
+        <v>0.99122626408360404</v>
       </c>
       <c r="D12">
-        <v>0.99122626408360404</v>
+        <v>0.92837409460002085</v>
       </c>
       <c r="E12">
-        <v>0.91962397535184026</v>
+        <v>0.9968227820470783</v>
       </c>
       <c r="F12">
-        <v>0.9968227820470783</v>
+        <v>0.91137303514629431</v>
       </c>
       <c r="G12">
         <v>0.94028749938664102</v>
@@ -997,39 +979,42 @@
         <v>0.90554719448698884</v>
       </c>
       <c r="I12">
-        <v>0.96489092907264762</v>
+        <v>0.93817387871194036</v>
       </c>
       <c r="J12">
         <v>0.97571742784520454</v>
       </c>
       <c r="K12">
+        <v>0.94628640973260159</v>
+      </c>
+      <c r="L12">
         <v>0.8698313944026993</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>23</v>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.92542376473650234</v>
       </c>
       <c r="B13">
-        <v>0.92542376473650234</v>
+        <v>0.93227817448634553</v>
       </c>
       <c r="C13">
-        <v>0.93227817448634553</v>
+        <v>0.98443099826366287</v>
       </c>
       <c r="D13">
-        <v>0.98443099826366287</v>
+        <v>0.91224340250211555</v>
       </c>
       <c r="E13">
-        <v>0.92243521188950384</v>
+        <v>0.97057150856757768</v>
       </c>
       <c r="F13">
-        <v>0.97057150856757768</v>
+        <v>0.9143147762627003</v>
       </c>
       <c r="G13">
         <v>0.91441751903636614</v>
@@ -1038,39 +1023,42 @@
         <v>0.90702837128276181</v>
       </c>
       <c r="I13">
-        <v>0.93227817448634553</v>
+        <v>0.91544445995772461</v>
       </c>
       <c r="J13">
         <v>0.97607318390709219</v>
       </c>
       <c r="K13">
+        <v>0.94454888264332659</v>
+      </c>
+      <c r="L13">
         <v>0.85917472953325924</v>
       </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.27464179444738052</v>
       </c>
       <c r="B14">
-        <v>0.27464179444738052</v>
+        <v>0.25131761356332533</v>
       </c>
       <c r="C14">
-        <v>0.25131761356332533</v>
+        <v>0.4538591648133492</v>
       </c>
       <c r="D14">
-        <v>0.4538591648133492</v>
+        <v>0.67189447867719465</v>
       </c>
       <c r="E14">
-        <v>0.93765797992586453</v>
+        <v>0.43325816772550418</v>
       </c>
       <c r="F14">
-        <v>0.43325816772550418</v>
+        <v>0.39859171303898672</v>
       </c>
       <c r="G14">
         <v>0.37940935726273672</v>
@@ -1079,39 +1067,42 @@
         <v>0.35400137881365579</v>
       </c>
       <c r="I14">
-        <v>0.25131761356332533</v>
+        <v>0.30051501295763128</v>
       </c>
       <c r="J14">
         <v>0.72599976817978518</v>
       </c>
       <c r="K14">
+        <v>0.453755750989631</v>
+      </c>
+      <c r="L14">
         <v>1.6187216772736031</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.40104228256100222</v>
       </c>
       <c r="B15">
-        <v>0.40104228256100222</v>
+        <v>0.34974954911379141</v>
       </c>
       <c r="C15">
-        <v>0.34974954911379141</v>
+        <v>0.35955357914351033</v>
       </c>
       <c r="D15">
-        <v>0.35955357914351033</v>
+        <v>0.90708163151421617</v>
       </c>
       <c r="E15">
-        <v>0.80639099190921981</v>
+        <v>0.33605552261884991</v>
       </c>
       <c r="F15">
-        <v>0.33605552261884991</v>
+        <v>0.40417988477500472</v>
       </c>
       <c r="G15">
         <v>0.50012622359849301</v>
@@ -1120,39 +1111,42 @@
         <v>0.27825795382186691</v>
       </c>
       <c r="I15">
-        <v>0.34974954911379141</v>
+        <v>0.41723850119868577</v>
       </c>
       <c r="J15">
         <v>0.50582351070933174</v>
       </c>
       <c r="K15">
+        <v>0.5227664025830604</v>
+      </c>
+      <c r="L15">
         <v>1.0191381369215651</v>
       </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>26</v>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>0.45621907768080239</v>
       </c>
       <c r="B16" s="2">
-        <v>0.45621907768080239</v>
+        <v>0.43799508847264729</v>
       </c>
       <c r="C16" s="2">
-        <v>0.43799508847264729</v>
+        <v>0.40427688016318181</v>
       </c>
       <c r="D16" s="2">
-        <v>0.40427688016318181</v>
+        <v>0.85776415932502115</v>
       </c>
       <c r="E16" s="2">
-        <v>0.96857527504320451</v>
+        <v>0.38001534355132111</v>
       </c>
       <c r="F16" s="2">
-        <v>0.38001534355132111</v>
+        <v>0.39263990211914629</v>
       </c>
       <c r="G16" s="2">
         <v>0.51948746659878497</v>
@@ -1161,39 +1155,42 @@
         <v>0.31542951414009979</v>
       </c>
       <c r="I16" s="2">
-        <v>0.43799508847264729</v>
+        <v>0.48754950047582818</v>
       </c>
       <c r="J16" s="2">
         <v>0.35997696152122999</v>
       </c>
       <c r="K16" s="2">
+        <v>0.46371297136756751</v>
+      </c>
+      <c r="L16" s="2">
         <v>0.6988122367788161</v>
       </c>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>27</v>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.63605737362715542</v>
       </c>
       <c r="B17">
-        <v>0.63605737362715542</v>
+        <v>0.62418893831953037</v>
       </c>
       <c r="C17">
-        <v>0.62418893831953037</v>
+        <v>0.60977641031927754</v>
       </c>
       <c r="D17">
-        <v>0.60977641031927754</v>
+        <v>1.3368433160224831</v>
       </c>
       <c r="E17">
-        <v>1.403046185960573</v>
+        <v>0.59196246749333237</v>
       </c>
       <c r="F17">
-        <v>0.59196246749333237</v>
+        <v>0.60739595057150819</v>
       </c>
       <c r="G17">
         <v>0.67894153831232806</v>
@@ -1202,39 +1199,42 @@
         <v>0.52026125510431342</v>
       </c>
       <c r="I17">
-        <v>0.62418893831953037</v>
+        <v>0.64468713684475687</v>
       </c>
       <c r="J17">
         <v>0.61795524491217135</v>
       </c>
       <c r="K17">
+        <v>0.70747571193391268</v>
+      </c>
+      <c r="L17">
         <v>0.93838992800233301</v>
       </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>28</v>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1.219974302028346</v>
       </c>
       <c r="B18">
-        <v>1.219974302028346</v>
+        <v>1.2190641998303879</v>
       </c>
       <c r="C18">
-        <v>1.2190641998303879</v>
+        <v>1.076022915601285</v>
       </c>
       <c r="D18">
-        <v>1.076022915601285</v>
+        <v>3.769871237702251</v>
       </c>
       <c r="E18">
-        <v>4.0073072959965126</v>
+        <v>1.060699982094635</v>
       </c>
       <c r="F18">
-        <v>1.060699982094635</v>
+        <v>1.1875406449131289</v>
       </c>
       <c r="G18">
         <v>1.2122338366242931</v>
@@ -1243,39 +1243,42 @@
         <v>0.99237806417084351</v>
       </c>
       <c r="I18">
-        <v>1.2190641998303879</v>
+        <v>1.1690985507636129</v>
       </c>
       <c r="J18">
         <v>1.187554308096719</v>
       </c>
       <c r="K18">
+        <v>1.4914164883076479</v>
+      </c>
+      <c r="L18">
         <v>2.9940191417630619</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>29</v>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.27464179444738052</v>
       </c>
       <c r="B19">
-        <v>0.27464179444738052</v>
+        <v>0.25131761356332533</v>
       </c>
       <c r="C19">
-        <v>0.25131761356332533</v>
+        <v>0.35955357914351033</v>
       </c>
       <c r="D19">
-        <v>0.35955357914351033</v>
+        <v>0.25198495601383319</v>
       </c>
       <c r="E19">
-        <v>0.43805632942462702</v>
+        <v>0.33605552261884991</v>
       </c>
       <c r="F19">
-        <v>0.33605552261884991</v>
+        <v>0.39263990211914629</v>
       </c>
       <c r="G19">
         <v>0.1243332478882081</v>
@@ -1284,23 +1287,25 @@
         <v>0.27825795382186691</v>
       </c>
       <c r="I19">
-        <v>0.25131761356332533</v>
+        <v>0.1174010591161055</v>
       </c>
       <c r="J19">
         <v>0.35997696152122999</v>
       </c>
       <c r="K19">
+        <v>0.29646130615408012</v>
+      </c>
+      <c r="L19">
         <v>0.6988122367788161</v>
       </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
-        <v>5</v>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>